<commit_message>
updated 2 sex GOA model
</commit_message>
<xml_diff>
--- a/GOA/Data/ATF 2018/ATF_fsh_length_comp.xlsx
+++ b/GOA/Data/ATF 2018/ATF_fsh_length_comp.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Adams\Documents\GitHub\RceattleRuns\GOA\ATF 2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Adams\Documents\GitHub\RceattleRuns\GOA\Data\ATF 2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="females" sheetId="1" r:id="rId1"/>
     <sheet name="males" sheetId="2" r:id="rId2"/>
+    <sheet name="sample_size" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,10 +23,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -344,7 +341,7 @@
   <dimension ref="A1:AB39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="C39" sqref="C1:AB39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3712,8 +3709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C1:AB39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7075,4 +7072,409 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>females!A1</f>
+        <v>1977</v>
+      </c>
+      <c r="B1">
+        <f>females!B1+males!B1</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>females!A2</f>
+        <v>1978</v>
+      </c>
+      <c r="B2">
+        <f>females!B2+males!B2</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>females!A3</f>
+        <v>1979</v>
+      </c>
+      <c r="B3">
+        <f>females!B3+males!B3</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>females!A4</f>
+        <v>1980</v>
+      </c>
+      <c r="B4">
+        <f>females!B4+males!B4</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>females!A5</f>
+        <v>1981</v>
+      </c>
+      <c r="B5">
+        <f>females!B5+males!B5</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>females!A6</f>
+        <v>1982</v>
+      </c>
+      <c r="B6">
+        <f>females!B6+males!B6</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>females!A7</f>
+        <v>1983</v>
+      </c>
+      <c r="B7">
+        <f>females!B7+males!B7</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>females!A8</f>
+        <v>1984</v>
+      </c>
+      <c r="B8">
+        <f>females!B8+males!B8</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>females!A9</f>
+        <v>1985</v>
+      </c>
+      <c r="B9">
+        <f>females!B9+males!B9</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>females!A10</f>
+        <v>1986</v>
+      </c>
+      <c r="B10">
+        <f>females!B10+males!B10</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>females!A11</f>
+        <v>1987</v>
+      </c>
+      <c r="B11">
+        <f>females!B11+males!B11</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>females!A12</f>
+        <v>1988</v>
+      </c>
+      <c r="B12">
+        <f>females!B12+males!B12</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>females!A13</f>
+        <v>1990</v>
+      </c>
+      <c r="B13">
+        <f>females!B13+males!B13</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>females!A14</f>
+        <v>1991</v>
+      </c>
+      <c r="B14">
+        <f>females!B14+males!B14</f>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>females!A15</f>
+        <v>1992</v>
+      </c>
+      <c r="B15">
+        <f>females!B15+males!B15</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>females!A16</f>
+        <v>1993</v>
+      </c>
+      <c r="B16">
+        <f>females!B16+males!B16</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>females!A17</f>
+        <v>1995</v>
+      </c>
+      <c r="B17">
+        <f>females!B17+males!B17</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>females!A18</f>
+        <v>1996</v>
+      </c>
+      <c r="B18">
+        <f>females!B18+males!B18</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>females!A19</f>
+        <v>1997</v>
+      </c>
+      <c r="B19">
+        <f>females!B19+males!B19</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>females!A20</f>
+        <v>1998</v>
+      </c>
+      <c r="B20">
+        <f>females!B20+males!B20</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>females!A21</f>
+        <v>1999</v>
+      </c>
+      <c r="B21">
+        <f>females!B21+males!B21</f>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>females!A22</f>
+        <v>2000</v>
+      </c>
+      <c r="B22">
+        <f>females!B22+males!B22</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>females!A23</f>
+        <v>2001</v>
+      </c>
+      <c r="B23">
+        <f>females!B23+males!B23</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>females!A24</f>
+        <v>2002</v>
+      </c>
+      <c r="B24">
+        <f>females!B24+males!B24</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>females!A25</f>
+        <v>2003</v>
+      </c>
+      <c r="B25">
+        <f>females!B25+males!B25</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>females!A26</f>
+        <v>2004</v>
+      </c>
+      <c r="B26">
+        <f>females!B26+males!B26</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f>females!A27</f>
+        <v>2005</v>
+      </c>
+      <c r="B27">
+        <f>females!B27+males!B27</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f>females!A28</f>
+        <v>2006</v>
+      </c>
+      <c r="B28">
+        <f>females!B28+males!B28</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f>females!A29</f>
+        <v>2007</v>
+      </c>
+      <c r="B29">
+        <f>females!B29+males!B29</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>females!A30</f>
+        <v>2008</v>
+      </c>
+      <c r="B30">
+        <f>females!B30+males!B30</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>females!A31</f>
+        <v>2009</v>
+      </c>
+      <c r="B31">
+        <f>females!B31+males!B31</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f>females!A32</f>
+        <v>2010</v>
+      </c>
+      <c r="B32">
+        <f>females!B32+males!B32</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>females!A33</f>
+        <v>2011</v>
+      </c>
+      <c r="B33">
+        <f>females!B33+males!B33</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f>females!A34</f>
+        <v>2012</v>
+      </c>
+      <c r="B34">
+        <f>females!B34+males!B34</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f>females!A35</f>
+        <v>2013</v>
+      </c>
+      <c r="B35">
+        <f>females!B35+males!B35</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>females!A36</f>
+        <v>2014</v>
+      </c>
+      <c r="B36">
+        <f>females!B36+males!B36</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>females!A37</f>
+        <v>2015</v>
+      </c>
+      <c r="B37">
+        <f>females!B37+males!B37</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>females!A38</f>
+        <v>2016</v>
+      </c>
+      <c r="B38">
+        <f>females!B38+males!B38</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>females!A39</f>
+        <v>2017</v>
+      </c>
+      <c r="B39">
+        <f>females!B39+males!B39</f>
+        <v>332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>